<commit_message>
Add sensor type registration form
</commit_message>
<xml_diff>
--- a/doc/Gateway-model-registration-form.xlsx
+++ b/doc/Gateway-model-registration-form.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>* Gateway infomation</t>
   </si>
@@ -35,9 +35,6 @@
     <t xml:space="preserve">   (Please contact us if you can not use the above three items.)</t>
   </si>
   <si>
-    <t>3. Sensor infomation</t>
-  </si>
-  <si>
     <t>4. Actuator infomation</t>
   </si>
   <si>
@@ -72,10 +69,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>4. Report interval (Minium is 60 second):</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">   4.1. Whether Thing+ Portal displays the report interval: </t>
     </r>
@@ -193,7 +186,415 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">4. Report interval (Minium is 60 seconds): </t>
+      <t xml:space="preserve">   4.1. Whether the report interval can be changed: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Yes</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   4.1. Whether Thing+ Portal displays the report interval: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Yes</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Gateway name: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Dali Gateway GA1000</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Device name: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Dali D100 Sensor Node</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. Whether the device is able to automatically detect what sensors are attached to it: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Yes</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   * Sensor type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>temperature</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Data format: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>number</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Decimal precision: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Unit: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Min/Max(opt):</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   * Sensor type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>humidity</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">     (In the parameter, specify the content of the required value, unit, and whether it is required.)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Data format: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>number</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Unit: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>%</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Min/Max(opt): </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-100/200</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Min/Max(opt): </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0/100</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Sensor infomation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. Actuator infomation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   * Sensor type:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">     - Command:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       . Parameter:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   * Sensor type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>led</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       . Parameter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">         1) Duration(opt)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">            - Unit: second</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">            - Min/Max: 0/180</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">       . Parameter: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>No</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Command: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>On</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Command: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Off</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">     - Command: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Blink</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">         1) Interval</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">         2) Duration(opt)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">            - Min/Max: 0/10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">            - Data format: number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Device(Sensor node) information (If you have multiple devices in use, you should describe all of them here)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Would you please fill each qustion? </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hi Partners. To register your gateway with the sensors, we need to get the information as mentioned below.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gateway Model Registration From</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Sensor infomation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. How many the devices can be connected in a gateway: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. How many the devices can be connected in a gateway:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. Report interval (Minimum is 60 second):</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. Report interval (Minimum is 60 seconds): </t>
     </r>
     <r>
       <rPr>
@@ -208,395 +609,15 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">   4.1. Whether the report interval can be changed: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Yes</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   4.1. Whether Thing+ Portal displays the report interval: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Yes</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. Gateway name: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Dali Gateway GA1000</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Device name: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Dali D100 Sensor Node</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. Whether the device is able to automatically detect what sensors are attached to it: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Yes</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   * Sensor type: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>temperature</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Data format: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>number</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Decimal precision: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Unit: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>°C</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">     - Min/Max(opt):</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   * Sensor type: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>humidity</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">     (In the parameter, specify the content of the required value, unit, and whether it is required.)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Data format: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>number</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Unit: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>%</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Min/Max(opt): </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>-100/200</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Min/Max(opt): </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>0/100</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4. Sensor infomation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5. Actuator infomation</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">   * Sensor type:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">     - Command:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">       . Parameter:</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">   * Sensor type: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>led</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">       . Parameter</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">         1) Duration(opt)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">            - Unit: second</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">            - Min/Max: 0/180</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">            - Description : The LED will turn off after the duration. The parameter is optional; if not, the LED remains on.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">       . Parameter: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>No</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Command: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>On</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Command: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Off</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">     - Command: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Blink</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">         1) Interval</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">         2) Duration(opt)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">            - Min/Max: 0/10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">            - Data format: number</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>* Device(Sensor node) information (If you have multiple devices in use, you should describe all of them here)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">            - Description : The LED will turn off after the duration. The parameter is optional; if not, the LED remains on.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">            - Description : The LED will rotate between on and off during the specified interval.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Would you please fill each qustion? </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hi Partners. To register your gateway with the sensors, we need to get the information as mentioned below.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gateway Model Registration From</t>
+    <t xml:space="preserve">            - Description: The LED will turn off after the duration. The parameter is optional; if not, the LED remains on.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">            - Description: The LED will rotate between on and off during the specified interval.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">            - Description: The LED will turn off after the duration. The parameter is optional; if not, the LED remains on.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1141,10 +1162,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C80"/>
+  <dimension ref="B1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1156,22 +1177,22 @@
   <sheetData>
     <row r="1" spans="2:3" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -1182,19 +1203,19 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="9"/>
     </row>
@@ -1212,19 +1233,19 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="9"/>
     </row>
@@ -1234,384 +1255,396 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C16" s="9"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="9"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" s="9"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="C19" s="9"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C21" s="9"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C22" s="9"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C23" s="9"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C24" s="9"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C28" s="9"/>
     </row>
-    <row r="29" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="10"/>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="2:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B32" s="12" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="13"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C34" s="15"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C35" s="15"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="14" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" s="15"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="14" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C38" s="15"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="14" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C39" s="15"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C40" s="15"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B41" s="14"/>
+      <c r="B41" s="14" t="s">
+        <v>20</v>
+      </c>
       <c r="C41" s="15"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="B42" s="14"/>
       <c r="C42" s="15"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="14" t="s">
-        <v>26</v>
+      <c r="B43" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="C43" s="15"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C44" s="15"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C45" s="15"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" s="14" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C46" s="15"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" s="14" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="C47" s="15"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" s="14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C48" s="15"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C49" s="15"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="14" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C50" s="15"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C51" s="15"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C52" s="15"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C53" s="15"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C54" s="15"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C55" s="15"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" s="14" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C56" s="15"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" s="14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C57" s="15"/>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" s="14" t="s">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="C58" s="15"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C59" s="15"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B60" s="17" t="s">
-        <v>46</v>
+      <c r="B60" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="C60" s="15"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B61" s="17" t="s">
-        <v>57</v>
+      <c r="B61" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="C61" s="15"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C62" s="15"/>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" s="17" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C63" s="15"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" s="17" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C64" s="15"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B65" s="14" t="s">
-        <v>52</v>
+      <c r="B65" s="17" t="s">
+        <v>45</v>
       </c>
       <c r="C65" s="15"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B66" s="14" t="s">
-        <v>50</v>
+      <c r="B66" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="C66" s="15"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C67" s="15"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C68" s="15"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B69" s="17" t="s">
-        <v>54</v>
+      <c r="B69" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="C69" s="15"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="17" t="s">
-        <v>57</v>
+      <c r="B70" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="C70" s="15"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" s="17" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C71" s="15"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B72" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C72" s="15"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B73" s="17" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C73" s="15"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B74" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C74" s="15"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B75" s="17" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C75" s="15"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" s="17" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C76" s="15"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B77" s="17" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C77" s="15"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" s="17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C78" s="15"/>
     </row>
-    <row r="79" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C79" s="19"/>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C79" s="15"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="1"/>
+      <c r="B80" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="15"/>
+    </row>
+    <row r="81" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B81" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C81" s="19"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>